<commit_message>
refactoring this entire repo.  Use a single utilities file.  Use a common database cxn found in utilities file.   Common LL connection values
</commit_message>
<xml_diff>
--- a/docs/masterPriceList.xlsx
+++ b/docs/masterPriceList.xlsx
@@ -1551,13 +1551,13 @@
         <v>29.15</v>
       </c>
       <c r="L2" s="1">
-        <v>32.74</v>
+        <v>32.53</v>
       </c>
       <c r="M2" s="3">
         <v>0.38</v>
       </c>
       <c r="N2" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -1613,13 +1613,13 @@
         <v>48.8</v>
       </c>
       <c r="L3" s="1">
-        <v>54.81</v>
+        <v>54.45</v>
       </c>
       <c r="M3" s="3">
         <v>0.38</v>
       </c>
       <c r="N3" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -1675,13 +1675,13 @@
         <v>9.87</v>
       </c>
       <c r="L4" s="1">
-        <v>11.08</v>
+        <v>11.01</v>
       </c>
       <c r="M4" s="3">
         <v>0.38</v>
       </c>
       <c r="N4" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -1737,13 +1737,13 @@
         <v>20.99</v>
       </c>
       <c r="L5" s="1">
-        <v>23.58</v>
+        <v>23.42</v>
       </c>
       <c r="M5" s="3">
         <v>0.38</v>
       </c>
       <c r="N5" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -1799,13 +1799,13 @@
         <v>25.56</v>
       </c>
       <c r="L6" s="1">
-        <v>28.71</v>
+        <v>28.53</v>
       </c>
       <c r="M6" s="3">
         <v>0.38</v>
       </c>
       <c r="N6" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -1861,13 +1861,13 @@
         <v>20.99</v>
       </c>
       <c r="L7" s="1">
-        <v>23.58</v>
+        <v>23.42</v>
       </c>
       <c r="M7" s="3">
         <v>0.38</v>
       </c>
       <c r="N7" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -1923,13 +1923,13 @@
         <v>25.65</v>
       </c>
       <c r="L8" s="1">
-        <v>28.81</v>
+        <v>28.63</v>
       </c>
       <c r="M8" s="3">
         <v>0.38</v>
       </c>
       <c r="N8" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -1985,13 +1985,13 @@
         <v>13.45</v>
       </c>
       <c r="L9" s="1">
-        <v>15.11</v>
+        <v>15.02</v>
       </c>
       <c r="M9" s="3">
         <v>0.38</v>
       </c>
       <c r="N9" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O9">
         <v>1</v>
@@ -2047,13 +2047,13 @@
         <v>19.24</v>
       </c>
       <c r="L10" s="1">
-        <v>21.61</v>
+        <v>21.47</v>
       </c>
       <c r="M10" s="3">
         <v>0.38</v>
       </c>
       <c r="N10" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O10">
         <v>1</v>
@@ -2109,13 +2109,13 @@
         <v>39.36</v>
       </c>
       <c r="L11" s="1">
-        <v>44.2</v>
+        <v>43.92</v>
       </c>
       <c r="M11" s="3">
         <v>0.38</v>
       </c>
       <c r="N11" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O11">
         <v>1</v>
@@ -2171,13 +2171,13 @@
         <v>29.74</v>
       </c>
       <c r="L12" s="1">
-        <v>33.4</v>
+        <v>33.18</v>
       </c>
       <c r="M12" s="3">
         <v>0.38</v>
       </c>
       <c r="N12" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O12">
         <v>1</v>
@@ -2239,7 +2239,7 @@
         <v>0.38</v>
       </c>
       <c r="N13" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O13">
         <v>1</v>
@@ -2295,13 +2295,13 @@
         <v>16.59</v>
       </c>
       <c r="L14" s="1">
-        <v>18.64</v>
+        <v>18.52</v>
       </c>
       <c r="M14" s="3">
         <v>0.38</v>
       </c>
       <c r="N14" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O14">
         <v>1</v>
@@ -2357,13 +2357,13 @@
         <v>21.21</v>
       </c>
       <c r="L15" s="1">
-        <v>23.83</v>
+        <v>23.67</v>
       </c>
       <c r="M15" s="3">
         <v>0.38</v>
       </c>
       <c r="N15" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O15">
         <v>1</v>
@@ -2419,13 +2419,13 @@
         <v>23.43</v>
       </c>
       <c r="L16" s="1">
-        <v>26.32</v>
+        <v>26.15</v>
       </c>
       <c r="M16" s="3">
         <v>0.38</v>
       </c>
       <c r="N16" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O16">
         <v>1</v>
@@ -2481,13 +2481,13 @@
         <v>38.62</v>
       </c>
       <c r="L17" s="1">
-        <v>43.37</v>
+        <v>43.09</v>
       </c>
       <c r="M17" s="3">
         <v>0.38</v>
       </c>
       <c r="N17" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O17">
         <v>1</v>
@@ -2543,13 +2543,13 @@
         <v>64.58</v>
       </c>
       <c r="L18" s="1">
-        <v>72.54</v>
+        <v>72.07</v>
       </c>
       <c r="M18" s="3">
         <v>0.38</v>
       </c>
       <c r="N18" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O18">
         <v>1</v>
@@ -2605,13 +2605,13 @@
         <v>53.3</v>
       </c>
       <c r="L19" s="1">
-        <v>59.86</v>
+        <v>59.47</v>
       </c>
       <c r="M19" s="3">
         <v>0.38</v>
       </c>
       <c r="N19" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O19">
         <v>1</v>
@@ -2667,13 +2667,13 @@
         <v>42.71</v>
       </c>
       <c r="L20" s="1">
-        <v>47.97</v>
+        <v>47.66</v>
       </c>
       <c r="M20" s="3">
         <v>0.38</v>
       </c>
       <c r="N20" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O20">
         <v>1</v>
@@ -2729,13 +2729,13 @@
         <v>37.32</v>
       </c>
       <c r="L21" s="1">
-        <v>41.91</v>
+        <v>41.64</v>
       </c>
       <c r="M21" s="3">
         <v>0.38</v>
       </c>
       <c r="N21" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O21">
         <v>1</v>
@@ -2791,13 +2791,13 @@
         <v>29.15</v>
       </c>
       <c r="L22" s="1">
-        <v>32.74</v>
+        <v>32.53</v>
       </c>
       <c r="M22" s="3">
         <v>0.38</v>
       </c>
       <c r="N22" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O22">
         <v>1</v>
@@ -2853,13 +2853,13 @@
         <v>13.9</v>
       </c>
       <c r="L23" s="1">
-        <v>15.62</v>
+        <v>15.52</v>
       </c>
       <c r="M23" s="3">
         <v>0.38</v>
       </c>
       <c r="N23" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O23">
         <v>1</v>
@@ -2915,13 +2915,13 @@
         <v>12.83</v>
       </c>
       <c r="L24" s="1">
-        <v>14.41</v>
+        <v>14.31</v>
       </c>
       <c r="M24" s="3">
         <v>0.38</v>
       </c>
       <c r="N24" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O24">
         <v>1</v>
@@ -2977,13 +2977,13 @@
         <v>22.74</v>
       </c>
       <c r="L25" s="1">
-        <v>25.54</v>
+        <v>25.38</v>
       </c>
       <c r="M25" s="3">
         <v>0.38</v>
       </c>
       <c r="N25" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O25">
         <v>1</v>
@@ -3039,13 +3039,13 @@
         <v>10.76</v>
       </c>
       <c r="L26" s="1">
-        <v>12.09</v>
+        <v>12.01</v>
       </c>
       <c r="M26" s="3">
         <v>0.38</v>
       </c>
       <c r="N26" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O26">
         <v>1</v>
@@ -3101,13 +3101,13 @@
         <v>23.23</v>
       </c>
       <c r="L27" s="1">
-        <v>26.09</v>
+        <v>25.93</v>
       </c>
       <c r="M27" s="3">
         <v>0.38</v>
       </c>
       <c r="N27" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O27">
         <v>1</v>
@@ -3163,13 +3163,13 @@
         <v>10.76</v>
       </c>
       <c r="L28" s="1">
-        <v>12.09</v>
+        <v>12.01</v>
       </c>
       <c r="M28" s="3">
         <v>0.38</v>
       </c>
       <c r="N28" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O28">
         <v>1</v>
@@ -3225,13 +3225,13 @@
         <v>34.51</v>
       </c>
       <c r="L29" s="1">
-        <v>38.76</v>
+        <v>38.51</v>
       </c>
       <c r="M29" s="3">
         <v>0.38</v>
       </c>
       <c r="N29" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O29">
         <v>1</v>
@@ -3287,13 +3287,13 @@
         <v>23.32</v>
       </c>
       <c r="L30" s="1">
-        <v>26.2</v>
+        <v>26.03</v>
       </c>
       <c r="M30" s="3">
         <v>0.38</v>
       </c>
       <c r="N30" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O30">
         <v>1</v>
@@ -3349,13 +3349,13 @@
         <v>13.88</v>
       </c>
       <c r="L31" s="1">
-        <v>15.59</v>
+        <v>15.49</v>
       </c>
       <c r="M31" s="3">
         <v>0.38</v>
       </c>
       <c r="N31" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O31">
         <v>1</v>
@@ -3411,13 +3411,13 @@
         <v>12.83</v>
       </c>
       <c r="L32" s="1">
-        <v>14.41</v>
+        <v>14.31</v>
       </c>
       <c r="M32" s="3">
         <v>0.38</v>
       </c>
       <c r="N32" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O32">
         <v>1</v>
@@ -3473,13 +3473,13 @@
         <v>32.52</v>
       </c>
       <c r="L33" s="1">
-        <v>36.52</v>
+        <v>36.29</v>
       </c>
       <c r="M33" s="3">
         <v>0.38</v>
       </c>
       <c r="N33" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O33">
         <v>1</v>
@@ -3535,13 +3535,13 @@
         <v>12.78</v>
       </c>
       <c r="L34" s="1">
-        <v>14.36</v>
+        <v>14.26</v>
       </c>
       <c r="M34" s="3">
         <v>0.38</v>
       </c>
       <c r="N34" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O34">
         <v>1</v>
@@ -3597,13 +3597,13 @@
         <v>23.32</v>
       </c>
       <c r="L35" s="1">
-        <v>26.2</v>
+        <v>26.03</v>
       </c>
       <c r="M35" s="3">
         <v>0.38</v>
       </c>
       <c r="N35" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O35">
         <v>1</v>
@@ -3659,13 +3659,13 @@
         <v>42.61</v>
       </c>
       <c r="L36" s="1">
-        <v>47.86</v>
+        <v>47.55</v>
       </c>
       <c r="M36" s="3">
         <v>0.38</v>
       </c>
       <c r="N36" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O36">
         <v>1</v>
@@ -3721,13 +3721,13 @@
         <v>15.25</v>
       </c>
       <c r="L37" s="1">
-        <v>17.13</v>
+        <v>17.02</v>
       </c>
       <c r="M37" s="3">
         <v>0.38</v>
       </c>
       <c r="N37" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O37">
         <v>1</v>
@@ -3783,13 +3783,13 @@
         <v>22.42</v>
       </c>
       <c r="L38" s="1">
-        <v>25.19</v>
+        <v>25.03</v>
       </c>
       <c r="M38" s="3">
         <v>0.38</v>
       </c>
       <c r="N38" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O38">
         <v>1</v>
@@ -3845,13 +3845,13 @@
         <v>12.56</v>
       </c>
       <c r="L39" s="1">
-        <v>14.11</v>
+        <v>14.01</v>
       </c>
       <c r="M39" s="3">
         <v>0.38</v>
       </c>
       <c r="N39" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O39">
         <v>1</v>
@@ -3907,13 +3907,13 @@
         <v>17.94</v>
       </c>
       <c r="L40" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M40" s="3">
         <v>0.38</v>
       </c>
       <c r="N40" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O40">
         <v>1</v>
@@ -3969,13 +3969,13 @@
         <v>14.8</v>
       </c>
       <c r="L41" s="1">
-        <v>16.62</v>
+        <v>16.52</v>
       </c>
       <c r="M41" s="3">
         <v>0.38</v>
       </c>
       <c r="N41" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O41">
         <v>1</v>
@@ -4031,13 +4031,13 @@
         <v>14.8</v>
       </c>
       <c r="L42" s="1">
-        <v>16.62</v>
+        <v>16.52</v>
       </c>
       <c r="M42" s="3">
         <v>0.38</v>
       </c>
       <c r="N42" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O42">
         <v>1</v>
@@ -4093,13 +4093,13 @@
         <v>14.8</v>
       </c>
       <c r="L43" s="1">
-        <v>16.62</v>
+        <v>16.52</v>
       </c>
       <c r="M43" s="3">
         <v>0.38</v>
       </c>
       <c r="N43" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O43">
         <v>1</v>
@@ -4155,13 +4155,13 @@
         <v>21.53</v>
       </c>
       <c r="L44" s="1">
-        <v>24.18</v>
+        <v>24.02</v>
       </c>
       <c r="M44" s="3">
         <v>0.38</v>
       </c>
       <c r="N44" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O44">
         <v>1</v>
@@ -4217,13 +4217,13 @@
         <v>14.8</v>
       </c>
       <c r="L45" s="1">
-        <v>16.62</v>
+        <v>16.52</v>
       </c>
       <c r="M45" s="3">
         <v>0.38</v>
       </c>
       <c r="N45" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O45">
         <v>1</v>
@@ -4279,13 +4279,13 @@
         <v>17.94</v>
       </c>
       <c r="L46" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M46" s="3">
         <v>0.38</v>
       </c>
       <c r="N46" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O46">
         <v>1</v>
@@ -4341,13 +4341,13 @@
         <v>17.94</v>
       </c>
       <c r="L47" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M47" s="3">
         <v>0.38</v>
       </c>
       <c r="N47" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O47">
         <v>1</v>
@@ -4403,13 +4403,13 @@
         <v>17.94</v>
       </c>
       <c r="L48" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M48" s="3">
         <v>0.38</v>
       </c>
       <c r="N48" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O48">
         <v>1</v>
@@ -4465,13 +4465,13 @@
         <v>17.94</v>
       </c>
       <c r="L49" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M49" s="3">
         <v>0.38</v>
       </c>
       <c r="N49" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O49">
         <v>1</v>
@@ -4527,13 +4527,13 @@
         <v>13.45</v>
       </c>
       <c r="L50" s="1">
-        <v>15.11</v>
+        <v>15.02</v>
       </c>
       <c r="M50" s="3">
         <v>0.38</v>
       </c>
       <c r="N50" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O50">
         <v>1</v>
@@ -4589,13 +4589,13 @@
         <v>17.94</v>
       </c>
       <c r="L51" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M51" s="3">
         <v>0.38</v>
       </c>
       <c r="N51" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O51">
         <v>1</v>
@@ -4651,13 +4651,13 @@
         <v>17.94</v>
       </c>
       <c r="L52" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M52" s="3">
         <v>0.38</v>
       </c>
       <c r="N52" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O52">
         <v>1</v>
@@ -4713,13 +4713,13 @@
         <v>15.25</v>
       </c>
       <c r="L53" s="1">
-        <v>17.13</v>
+        <v>17.02</v>
       </c>
       <c r="M53" s="3">
         <v>0.38</v>
       </c>
       <c r="N53" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O53">
         <v>1</v>
@@ -4775,13 +4775,13 @@
         <v>17.94</v>
       </c>
       <c r="L54" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M54" s="3">
         <v>0.38</v>
       </c>
       <c r="N54" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O54">
         <v>1</v>
@@ -4837,13 +4837,13 @@
         <v>8.97</v>
       </c>
       <c r="L55" s="1">
-        <v>10.08</v>
+        <v>10.01</v>
       </c>
       <c r="M55" s="3">
         <v>0.38</v>
       </c>
       <c r="N55" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O55">
         <v>1</v>
@@ -4899,13 +4899,13 @@
         <v>13.45</v>
       </c>
       <c r="L56" s="1">
-        <v>15.11</v>
+        <v>15.02</v>
       </c>
       <c r="M56" s="3">
         <v>0.38</v>
       </c>
       <c r="N56" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O56">
         <v>1</v>
@@ -4961,13 +4961,13 @@
         <v>8.97</v>
       </c>
       <c r="L57" s="1">
-        <v>10.08</v>
+        <v>10.01</v>
       </c>
       <c r="M57" s="3">
         <v>0.38</v>
       </c>
       <c r="N57" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O57">
         <v>1</v>
@@ -5023,13 +5023,13 @@
         <v>14.35</v>
       </c>
       <c r="L58" s="1">
-        <v>16.12</v>
+        <v>16.02</v>
       </c>
       <c r="M58" s="3">
         <v>0.38</v>
       </c>
       <c r="N58" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O58">
         <v>1</v>
@@ -5085,13 +5085,13 @@
         <v>8.97</v>
       </c>
       <c r="L59" s="1">
-        <v>10.08</v>
+        <v>10.01</v>
       </c>
       <c r="M59" s="3">
         <v>0.38</v>
       </c>
       <c r="N59" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O59">
         <v>1</v>
@@ -5147,13 +5147,13 @@
         <v>19.73</v>
       </c>
       <c r="L60" s="1">
-        <v>22.17</v>
+        <v>22.02</v>
       </c>
       <c r="M60" s="3">
         <v>0.38</v>
       </c>
       <c r="N60" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O60">
         <v>1</v>
@@ -5209,13 +5209,13 @@
         <v>17.94</v>
       </c>
       <c r="L61" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M61" s="3">
         <v>0.38</v>
       </c>
       <c r="N61" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O61">
         <v>1</v>
@@ -5271,13 +5271,13 @@
         <v>17.94</v>
       </c>
       <c r="L62" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M62" s="3">
         <v>0.38</v>
       </c>
       <c r="N62" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O62">
         <v>1</v>
@@ -5333,13 +5333,13 @@
         <v>8.97</v>
       </c>
       <c r="L63" s="1">
-        <v>10.08</v>
+        <v>10.01</v>
       </c>
       <c r="M63" s="3">
         <v>0.38</v>
       </c>
       <c r="N63" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O63">
         <v>1</v>
@@ -5395,13 +5395,13 @@
         <v>19.38</v>
       </c>
       <c r="L64" s="1">
-        <v>21.76</v>
+        <v>21.62</v>
       </c>
       <c r="M64" s="3">
         <v>0.38</v>
       </c>
       <c r="N64" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O64">
         <v>1</v>
@@ -5457,13 +5457,13 @@
         <v>37.67</v>
       </c>
       <c r="L65" s="1">
-        <v>42.32</v>
+        <v>42.04</v>
       </c>
       <c r="M65" s="3">
         <v>0.38</v>
       </c>
       <c r="N65" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O65">
         <v>1</v>
@@ -5519,13 +5519,13 @@
         <v>8.1</v>
       </c>
       <c r="L66" s="1">
-        <v>9.09</v>
+        <v>9.03</v>
       </c>
       <c r="M66" s="3">
         <v>0.38</v>
       </c>
       <c r="N66" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O66">
         <v>1</v>
@@ -5581,13 +5581,13 @@
         <v>23.62</v>
       </c>
       <c r="L67" s="1">
-        <v>26.54</v>
+        <v>26.36</v>
       </c>
       <c r="M67" s="3">
         <v>0.38</v>
       </c>
       <c r="N67" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O67">
         <v>1</v>
@@ -5643,13 +5643,13 @@
         <v>18.07</v>
       </c>
       <c r="L68" s="1">
-        <v>20.3</v>
+        <v>20.17</v>
       </c>
       <c r="M68" s="3">
         <v>0.38</v>
       </c>
       <c r="N68" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O68">
         <v>1</v>
@@ -5705,13 +5705,13 @@
         <v>27.38</v>
       </c>
       <c r="L69" s="1">
-        <v>30.75</v>
+        <v>30.56</v>
       </c>
       <c r="M69" s="3">
         <v>0.38</v>
       </c>
       <c r="N69" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O69">
         <v>1</v>
@@ -5767,13 +5767,13 @@
         <v>21.3</v>
       </c>
       <c r="L70" s="1">
-        <v>23.93</v>
+        <v>23.77</v>
       </c>
       <c r="M70" s="3">
         <v>0.38</v>
       </c>
       <c r="N70" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O70">
         <v>1</v>
@@ -5829,13 +5829,13 @@
         <v>38.35</v>
       </c>
       <c r="L71" s="1">
-        <v>43.07</v>
+        <v>42.79</v>
       </c>
       <c r="M71" s="3">
         <v>0.38</v>
       </c>
       <c r="N71" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O71">
         <v>1</v>
@@ -5891,13 +5891,13 @@
         <v>44.85</v>
       </c>
       <c r="L72" s="1">
-        <v>50.38</v>
+        <v>50.05</v>
       </c>
       <c r="M72" s="3">
         <v>0.38</v>
       </c>
       <c r="N72" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O72">
         <v>1</v>
@@ -5959,7 +5959,7 @@
         <v>0.38</v>
       </c>
       <c r="N73" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O73">
         <v>1</v>
@@ -6015,13 +6015,13 @@
         <v>19.29</v>
       </c>
       <c r="L74" s="1">
-        <v>21.66</v>
+        <v>21.52</v>
       </c>
       <c r="M74" s="3">
         <v>0.38</v>
       </c>
       <c r="N74" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O74">
         <v>1</v>
@@ -6077,13 +6077,13 @@
         <v>54</v>
       </c>
       <c r="L75" s="1">
-        <v>60.65</v>
+        <v>60.26</v>
       </c>
       <c r="M75" s="3">
         <v>0.38</v>
       </c>
       <c r="N75" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O75">
         <v>1</v>
@@ -6139,13 +6139,13 @@
         <v>10.76</v>
       </c>
       <c r="L76" s="1">
-        <v>12.09</v>
+        <v>12.01</v>
       </c>
       <c r="M76" s="3">
         <v>0.38</v>
       </c>
       <c r="N76" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O76">
         <v>1</v>
@@ -6201,13 +6201,13 @@
         <v>6.28</v>
       </c>
       <c r="L77" s="1">
-        <v>7.05</v>
+        <v>7.01</v>
       </c>
       <c r="M77" s="3">
         <v>0.38</v>
       </c>
       <c r="N77" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O77">
         <v>1</v>
@@ -6263,13 +6263,13 @@
         <v>19.38</v>
       </c>
       <c r="L78" s="1">
-        <v>21.76</v>
+        <v>21.62</v>
       </c>
       <c r="M78" s="3">
         <v>0.38</v>
       </c>
       <c r="N78" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O78">
         <v>1</v>
@@ -6325,13 +6325,13 @@
         <v>15.25</v>
       </c>
       <c r="L79" s="1">
-        <v>17.13</v>
+        <v>17.02</v>
       </c>
       <c r="M79" s="3">
         <v>0.38</v>
       </c>
       <c r="N79" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O79">
         <v>1</v>
@@ -6387,13 +6387,13 @@
         <v>10.76</v>
       </c>
       <c r="L80" s="1">
-        <v>12.09</v>
+        <v>12.01</v>
       </c>
       <c r="M80" s="3">
         <v>0.38</v>
       </c>
       <c r="N80" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O80">
         <v>1</v>
@@ -6449,13 +6449,13 @@
         <v>8.97</v>
       </c>
       <c r="L81" s="1">
-        <v>10.08</v>
+        <v>10.01</v>
       </c>
       <c r="M81" s="3">
         <v>0.38</v>
       </c>
       <c r="N81" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O81">
         <v>1</v>
@@ -6511,13 +6511,13 @@
         <v>20.59</v>
       </c>
       <c r="L82" s="1">
-        <v>23.12</v>
+        <v>22.97</v>
       </c>
       <c r="M82" s="3">
         <v>0.38</v>
       </c>
       <c r="N82" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O82">
         <v>1</v>
@@ -6573,13 +6573,13 @@
         <v>23.61</v>
       </c>
       <c r="L83" s="1">
-        <v>26.52</v>
+        <v>26.35</v>
       </c>
       <c r="M83" s="3">
         <v>0.38</v>
       </c>
       <c r="N83" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O83">
         <v>1</v>
@@ -6635,13 +6635,13 @@
         <v>41.93</v>
       </c>
       <c r="L84" s="1">
-        <v>47.1</v>
+        <v>46.8</v>
       </c>
       <c r="M84" s="3">
         <v>0.38</v>
       </c>
       <c r="N84" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O84">
         <v>1</v>
@@ -6697,13 +6697,13 @@
         <v>55.1</v>
       </c>
       <c r="L85" s="1">
-        <v>61.89</v>
+        <v>61.49</v>
       </c>
       <c r="M85" s="3">
         <v>0.38</v>
       </c>
       <c r="N85" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O85">
         <v>1</v>
@@ -6759,13 +6759,13 @@
         <v>41.89</v>
       </c>
       <c r="L86" s="1">
-        <v>47.05</v>
+        <v>46.75</v>
       </c>
       <c r="M86" s="3">
         <v>0.38</v>
       </c>
       <c r="N86" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O86">
         <v>1</v>
@@ -6827,7 +6827,7 @@
         <v>0.38</v>
       </c>
       <c r="N87" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O87">
         <v>1</v>
@@ -6883,13 +6883,13 @@
         <v>32.52</v>
       </c>
       <c r="L88" s="1">
-        <v>36.52</v>
+        <v>36.29</v>
       </c>
       <c r="M88" s="3">
         <v>0.38</v>
       </c>
       <c r="N88" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O88">
         <v>1</v>
@@ -6945,13 +6945,13 @@
         <v>13.66</v>
       </c>
       <c r="L89" s="1">
-        <v>15.34</v>
+        <v>15.24</v>
       </c>
       <c r="M89" s="3">
         <v>0.38</v>
       </c>
       <c r="N89" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O89">
         <v>1</v>
@@ -7007,13 +7007,13 @@
         <v>8.52</v>
       </c>
       <c r="L90" s="1">
-        <v>9.57</v>
+        <v>9.51</v>
       </c>
       <c r="M90" s="3">
         <v>0.38</v>
       </c>
       <c r="N90" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O90">
         <v>1</v>
@@ -7069,13 +7069,13 @@
         <v>8.52</v>
       </c>
       <c r="L91" s="1">
-        <v>9.57</v>
+        <v>9.51</v>
       </c>
       <c r="M91" s="3">
         <v>0.38</v>
       </c>
       <c r="N91" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O91">
         <v>1</v>
@@ -7131,13 +7131,13 @@
         <v>10.76</v>
       </c>
       <c r="L92" s="1">
-        <v>12.09</v>
+        <v>12.01</v>
       </c>
       <c r="M92" s="3">
         <v>0.38</v>
       </c>
       <c r="N92" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O92">
         <v>1</v>
@@ -7193,13 +7193,13 @@
         <v>24.22</v>
       </c>
       <c r="L93" s="1">
-        <v>27.2</v>
+        <v>27.03</v>
       </c>
       <c r="M93" s="3">
         <v>0.38</v>
       </c>
       <c r="N93" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O93">
         <v>1</v>
@@ -7255,13 +7255,13 @@
         <v>104.55</v>
       </c>
       <c r="L94" s="1">
-        <v>117.42</v>
+        <v>116.67</v>
       </c>
       <c r="M94" s="3">
         <v>0.38</v>
       </c>
       <c r="N94" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O94">
         <v>1</v>
@@ -7317,13 +7317,13 @@
         <v>17.38</v>
       </c>
       <c r="L95" s="1">
-        <v>19.52</v>
+        <v>19.39</v>
       </c>
       <c r="M95" s="3">
         <v>0.38</v>
       </c>
       <c r="N95" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O95">
         <v>1</v>
@@ -7379,13 +7379,13 @@
         <v>18.84</v>
       </c>
       <c r="L96" s="1">
-        <v>21.16</v>
+        <v>21.02</v>
       </c>
       <c r="M96" s="3">
         <v>0.38</v>
       </c>
       <c r="N96" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O96">
         <v>1</v>
@@ -7441,13 +7441,13 @@
         <v>44.4</v>
       </c>
       <c r="L97" s="1">
-        <v>49.87</v>
+        <v>49.55</v>
       </c>
       <c r="M97" s="3">
         <v>0.38</v>
       </c>
       <c r="N97" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O97">
         <v>1</v>
@@ -7503,13 +7503,13 @@
         <v>39.24</v>
       </c>
       <c r="L98" s="1">
-        <v>44.08</v>
+        <v>43.79</v>
       </c>
       <c r="M98" s="3">
         <v>0.38</v>
       </c>
       <c r="N98" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O98">
         <v>1</v>
@@ -7565,13 +7565,13 @@
         <v>33.19</v>
       </c>
       <c r="L99" s="1">
-        <v>37.28</v>
+        <v>37.04</v>
       </c>
       <c r="M99" s="3">
         <v>0.38</v>
       </c>
       <c r="N99" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O99">
         <v>1</v>
@@ -7627,13 +7627,13 @@
         <v>26.8</v>
       </c>
       <c r="L100" s="1">
-        <v>30.1</v>
+        <v>29.9</v>
       </c>
       <c r="M100" s="3">
         <v>0.38</v>
       </c>
       <c r="N100" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O100">
         <v>1</v>
@@ -7689,13 +7689,13 @@
         <v>58.13</v>
       </c>
       <c r="L101" s="1">
-        <v>65.29</v>
+        <v>64.86</v>
       </c>
       <c r="M101" s="3">
         <v>0.38</v>
       </c>
       <c r="N101" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O101">
         <v>1</v>
@@ -7751,13 +7751,13 @@
         <v>48.98</v>
       </c>
       <c r="L102" s="1">
-        <v>55.01</v>
+        <v>54.65</v>
       </c>
       <c r="M102" s="3">
         <v>0.38</v>
       </c>
       <c r="N102" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O102">
         <v>1</v>
@@ -7813,13 +7813,13 @@
         <v>37.67</v>
       </c>
       <c r="L103" s="1">
-        <v>42.32</v>
+        <v>42.04</v>
       </c>
       <c r="M103" s="3">
         <v>0.38</v>
       </c>
       <c r="N103" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O103">
         <v>1</v>
@@ -7875,13 +7875,13 @@
         <v>16.59</v>
       </c>
       <c r="L104" s="1">
-        <v>18.64</v>
+        <v>18.52</v>
       </c>
       <c r="M104" s="3">
         <v>0.38</v>
       </c>
       <c r="N104" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O104">
         <v>1</v>
@@ -7937,13 +7937,13 @@
         <v>10.76</v>
       </c>
       <c r="L105" s="1">
-        <v>12.09</v>
+        <v>12.01</v>
       </c>
       <c r="M105" s="3">
         <v>0.38</v>
       </c>
       <c r="N105" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O105">
         <v>1</v>
@@ -7999,13 +7999,13 @@
         <v>13.01</v>
       </c>
       <c r="L106" s="1">
-        <v>14.61</v>
+        <v>14.51</v>
       </c>
       <c r="M106" s="3">
         <v>0.38</v>
       </c>
       <c r="N106" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O106">
         <v>1</v>
@@ -8061,13 +8061,13 @@
         <v>15.7</v>
       </c>
       <c r="L107" s="1">
-        <v>17.63</v>
+        <v>17.52</v>
       </c>
       <c r="M107" s="3">
         <v>0.38</v>
       </c>
       <c r="N107" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O107">
         <v>1</v>
@@ -8123,13 +8123,13 @@
         <v>17.49</v>
       </c>
       <c r="L108" s="1">
-        <v>19.65</v>
+        <v>19.52</v>
       </c>
       <c r="M108" s="3">
         <v>0.38</v>
       </c>
       <c r="N108" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O108">
         <v>1</v>
@@ -8185,13 +8185,13 @@
         <v>13.9</v>
       </c>
       <c r="L109" s="1">
-        <v>15.62</v>
+        <v>15.52</v>
       </c>
       <c r="M109" s="3">
         <v>0.38</v>
       </c>
       <c r="N109" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O109">
         <v>1</v>
@@ -8247,13 +8247,13 @@
         <v>17.49</v>
       </c>
       <c r="L110" s="1">
-        <v>19.65</v>
+        <v>19.52</v>
       </c>
       <c r="M110" s="3">
         <v>0.38</v>
       </c>
       <c r="N110" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O110">
         <v>1</v>
@@ -8309,13 +8309,13 @@
         <v>17.49</v>
       </c>
       <c r="L111" s="1">
-        <v>19.65</v>
+        <v>19.52</v>
       </c>
       <c r="M111" s="3">
         <v>0.38</v>
       </c>
       <c r="N111" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O111">
         <v>1</v>
@@ -8371,13 +8371,13 @@
         <v>19.29</v>
       </c>
       <c r="L112" s="1">
-        <v>21.66</v>
+        <v>21.52</v>
       </c>
       <c r="M112" s="3">
         <v>0.38</v>
       </c>
       <c r="N112" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O112">
         <v>1</v>
@@ -8433,13 +8433,13 @@
         <v>19.29</v>
       </c>
       <c r="L113" s="1">
-        <v>21.66</v>
+        <v>21.52</v>
       </c>
       <c r="M113" s="3">
         <v>0.38</v>
       </c>
       <c r="N113" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O113">
         <v>1</v>
@@ -8495,13 +8495,13 @@
         <v>14.8</v>
       </c>
       <c r="L114" s="1">
-        <v>16.62</v>
+        <v>16.52</v>
       </c>
       <c r="M114" s="3">
         <v>0.38</v>
       </c>
       <c r="N114" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O114">
         <v>1</v>
@@ -8557,13 +8557,13 @@
         <v>17.94</v>
       </c>
       <c r="L115" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M115" s="3">
         <v>0.38</v>
       </c>
       <c r="N115" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O115">
         <v>1</v>
@@ -8619,13 +8619,13 @@
         <v>19.29</v>
       </c>
       <c r="L116" s="1">
-        <v>21.66</v>
+        <v>21.52</v>
       </c>
       <c r="M116" s="3">
         <v>0.38</v>
       </c>
       <c r="N116" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O116">
         <v>1</v>
@@ -8681,13 +8681,13 @@
         <v>16.15</v>
       </c>
       <c r="L117" s="1">
-        <v>18.14</v>
+        <v>18.02</v>
       </c>
       <c r="M117" s="3">
         <v>0.38</v>
       </c>
       <c r="N117" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O117">
         <v>1</v>
@@ -8743,13 +8743,13 @@
         <v>16.15</v>
       </c>
       <c r="L118" s="1">
-        <v>18.14</v>
+        <v>18.02</v>
       </c>
       <c r="M118" s="3">
         <v>0.38</v>
       </c>
       <c r="N118" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O118">
         <v>1</v>
@@ -8805,13 +8805,13 @@
         <v>17.94</v>
       </c>
       <c r="L119" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M119" s="3">
         <v>0.38</v>
       </c>
       <c r="N119" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O119">
         <v>1</v>
@@ -8867,13 +8867,13 @@
         <v>16.15</v>
       </c>
       <c r="L120" s="1">
-        <v>18.14</v>
+        <v>18.02</v>
       </c>
       <c r="M120" s="3">
         <v>0.38</v>
       </c>
       <c r="N120" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O120">
         <v>1</v>
@@ -8929,13 +8929,13 @@
         <v>17.94</v>
       </c>
       <c r="L121" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M121" s="3">
         <v>0.38</v>
       </c>
       <c r="N121" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O121">
         <v>1</v>
@@ -8991,13 +8991,13 @@
         <v>8.07</v>
       </c>
       <c r="L122" s="1">
-        <v>9.07</v>
+        <v>9.01</v>
       </c>
       <c r="M122" s="3">
         <v>0.38</v>
       </c>
       <c r="N122" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O122">
         <v>1</v>
@@ -9053,13 +9053,13 @@
         <v>17.49</v>
       </c>
       <c r="L123" s="1">
-        <v>19.65</v>
+        <v>19.52</v>
       </c>
       <c r="M123" s="3">
         <v>0.38</v>
       </c>
       <c r="N123" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O123">
         <v>1</v>
@@ -9115,13 +9115,13 @@
         <v>17.94</v>
       </c>
       <c r="L124" s="1">
-        <v>20.15</v>
+        <v>20.02</v>
       </c>
       <c r="M124" s="3">
         <v>0.38</v>
       </c>
       <c r="N124" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O124">
         <v>1</v>
@@ -9177,13 +9177,13 @@
         <v>14.8</v>
       </c>
       <c r="L125" s="1">
-        <v>16.62</v>
+        <v>16.52</v>
       </c>
       <c r="M125" s="3">
         <v>0.38</v>
       </c>
       <c r="N125" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O125">
         <v>1</v>
@@ -9239,13 +9239,13 @@
         <v>9.87</v>
       </c>
       <c r="L126" s="1">
-        <v>11.08</v>
+        <v>11.01</v>
       </c>
       <c r="M126" s="3">
         <v>0.38</v>
       </c>
       <c r="N126" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O126">
         <v>1</v>
@@ -9301,13 +9301,13 @@
         <v>15.25</v>
       </c>
       <c r="L127" s="1">
-        <v>17.13</v>
+        <v>17.02</v>
       </c>
       <c r="M127" s="3">
         <v>0.38</v>
       </c>
       <c r="N127" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O127">
         <v>1</v>
@@ -9363,13 +9363,13 @@
         <v>17.49</v>
       </c>
       <c r="L128" s="1">
-        <v>19.65</v>
+        <v>19.52</v>
       </c>
       <c r="M128" s="3">
         <v>0.38</v>
       </c>
       <c r="N128" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O128">
         <v>1</v>
@@ -9425,13 +9425,13 @@
         <v>16.15</v>
       </c>
       <c r="L129" s="1">
-        <v>18.14</v>
+        <v>18.02</v>
       </c>
       <c r="M129" s="3">
         <v>0.38</v>
       </c>
       <c r="N129" s="3">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="O129">
         <v>1</v>

</xml_diff>